<commit_message>
completed CAD HW5.2 and started HW5.3
</commit_message>
<xml_diff>
--- a/23FL/CAD/HW5.2/TU23FL-CAD-HW5.2.xlsx
+++ b/23FL/CAD/HW5.2/TU23FL-CAD-HW5.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\software\TU\23FL\CAD\HW5.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\software\TU\23FL\CAD\HW5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F9DC06-7F96-4013-B98F-A58ECF01D311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1E853D-6E68-4639-A08D-2D42BD3286D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{735F6D91-EA04-4AA0-81A9-2E9D99663C67}"/>
   </bookViews>
@@ -36,30 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Node</t>
   </si>
   <si>
-    <t>Value (N/m^2)</t>
-  </si>
-  <si>
-    <t>X(mm)</t>
-  </si>
-  <si>
-    <t>Y(mm)</t>
-  </si>
-  <si>
-    <t>Z(mm)</t>
-  </si>
-  <si>
-    <t>Top</t>
-  </si>
-  <si>
     <t>Centroid</t>
-  </si>
-  <si>
-    <t>Bottom</t>
   </si>
   <si>
     <t>Theory</t>
@@ -68,10 +50,37 @@
     <t>% Error</t>
   </si>
   <si>
-    <t>Sim Stress (N/m^2)</t>
+    <t>Value (psi)</t>
   </si>
   <si>
-    <t>Theory Stress (N/m^2)</t>
+    <t>X(in)</t>
+  </si>
+  <si>
+    <t>Y(in)</t>
+  </si>
+  <si>
+    <t>Z(in)</t>
+  </si>
+  <si>
+    <t>Sim Stress (psi)</t>
+  </si>
+  <si>
+    <t>Theory Stress (psi)</t>
+  </si>
+  <si>
+    <t>Outside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inside </t>
+  </si>
+  <si>
+    <t>Re-ran with refined mesh</t>
+  </si>
+  <si>
+    <t>Refined Sim Stress (psi)</t>
+  </si>
+  <si>
+    <t>Refined % Error</t>
   </si>
 </sst>
 </file>
@@ -79,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -147,17 +156,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -167,6 +173,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -234,7 +246,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" baseline="0"/>
-              <a:t> A-A (X = 50mm)</a:t>
+              <a:t> Q-Q</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -293,7 +305,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Value (N/m^2)</c:v>
+                  <c:v>Value (psi)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -329,31 +341,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.999998089999998</c:v>
+                  <c:v>3.5699999299999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.499998089999998</c:v>
+                  <c:v>3.63999987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.999996190000001</c:v>
+                  <c:v>3.7229833600000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.499998089999998</c:v>
+                  <c:v>3.8059663800000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.99999809</c:v>
+                  <c:v>3.8873774999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.49999905</c:v>
+                  <c:v>3.9687883899999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.9999976200000003</c:v>
+                  <c:v>4.0143942800000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4.1300001100000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,31 +377,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>61551512</c:v>
+                  <c:v>-13389.373</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39901732</c:v>
+                  <c:v>-10427.089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29080782</c:v>
+                  <c:v>-7509.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18256932</c:v>
+                  <c:v>-4329.308</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7432166.5</c:v>
+                  <c:v>-1315.2650000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3393733.5</c:v>
+                  <c:v>1263.357</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-14221835</c:v>
+                  <c:v>3834.5329999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-25048874</c:v>
+                  <c:v>5197.3469999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-46696284</c:v>
+                  <c:v>8563.3739999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,7 +458,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Height in Y (mm)</a:t>
+                  <a:t> Height in Y (in)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -529,8 +541,7 @@
         <c:axId val="749710760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="70000000"/>
-          <c:min val="-50000000"/>
+          <c:max val="15000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -569,7 +580,704 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>Stress in X (N/m^2)</a:t>
+                  <a:t>Stress in X (psi)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="749713576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Refined Nodal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Stress in X at Cross Section</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> Q-Q</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>Jakob Werle</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value (psi)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$13:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5037961000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5075919600000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5132603599999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.518929</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5282106400000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5453324300000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5645408600000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5975379900000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6529176200000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7133224</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7666833400000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8135280599999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8675391700000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9920864100000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0221362100000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.05218554</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0769815400000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1017770799999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.1376342800000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.1581554399999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.1690969500000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.1800375000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.1860923799999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.1921472499999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.1960735299999996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.1999998099999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-13381.357</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13219.883</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13046.843999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-12790.731</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-12522.108</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-12099.148999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-11326.541999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10483.416999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9087.8610000000008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6866.0330000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4565.4790000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2668.4749999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1133.2280000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>636.24800000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4580.3410000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5463.5150000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6350.9669999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7070.3389999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7785.4579999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8804.7759999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9378.8680000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9682.51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9986.1350000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10146.768</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10301.344999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10410.376</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10518.687</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7BB-453F-B825-F7C1F7A31312}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value (psi)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$13:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0" formatCode="#,##0.00">
+                  <c:v>-13389.373</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0.00">
+                  <c:v>-10427.089</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0.00">
+                  <c:v>-7509.11</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0.00">
+                  <c:v>-4329.308</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0.00">
+                  <c:v>-1315.2650000000001</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="#,##0.00">
+                  <c:v>1263.357</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="#,##0.00">
+                  <c:v>3834.5329999999999</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="#,##0.00">
+                  <c:v>5197.3469999999998</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0.00">
+                  <c:v>8563.3739999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A7BB-453F-B825-F7C1F7A31312}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="749713576"/>
+        <c:axId val="749710760"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="749713576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nodal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Height in Y (in)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="749710760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="749710760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="15000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Stress in X (psi)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -735,6 +1443,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1238,20 +1986,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>116204</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>54909</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>35522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>509644</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>141193</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1278,12 +2529,12 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>278130</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>990824</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9413</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="401905" cy="264560"/>
+    <xdr:ext cx="631327" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -1297,8 +2548,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2480310" y="2621280"/>
-          <a:ext cx="401905" cy="264560"/>
+          <a:off x="8427048" y="1847178"/>
+          <a:ext cx="631327" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1337,7 +2588,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Top</a:t>
+            <a:t>Outside</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1346,18 +2597,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>880559</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>113179</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="681533" cy="264560"/>
+    <xdr:ext cx="526170" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
+        <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E8474F8-2A9C-4071-9E72-05D8346EF132}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F58672F-8513-4FA2-9718-B7D0770F2D01}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,7 +2616,185 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4091940" y="2750820"/>
+          <a:off x="6931735" y="2318497"/>
+          <a:ext cx="526170" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Inside</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>170766</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76649</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>62753</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F5A04A8-E12F-EFE1-66EA-484A826FC7A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9059272" y="1980354"/>
+          <a:ext cx="1035436" cy="103940"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>593464</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>11082</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1143644</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>181759</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B10396E-3995-4D24-9D79-F873B7069686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6644640" y="2583953"/>
+          <a:ext cx="550180" cy="722006"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>491939</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166519</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="681533" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="TextBox 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73685D6D-C0B9-461D-8CC7-4DEED2AFC9DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9380445" y="2923166"/>
           <a:ext cx="681533" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1412,20 +2841,113 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1021304</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>128419</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>491939</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>115919</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C81F92-93A5-4351-B3A9-4520F21A55D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="31" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8457528" y="2701290"/>
+          <a:ext cx="922917" cy="355053"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>35859</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>4481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>490594</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>110152</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="35" name="Chart 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5007FCAB-2B85-43FD-908D-12C79945868A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>605342</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>54237</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="617348" cy="264560"/>
+    <xdr:ext cx="631327" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
+        <xdr:cNvPr id="42" name="TextBox 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F58672F-8513-4FA2-9718-B7D0770F2D01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8322F141-1B90-4176-8CE8-5152FFC14FF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,8 +2955,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2948940" y="3851910"/>
-          <a:ext cx="617348" cy="264560"/>
+          <a:off x="9574530" y="4648649"/>
+          <a:ext cx="631327" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1466,14 +2988,82 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Bottom</a:t>
+            <a:t>Outside</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>772983</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>140074</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="526170" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="TextBox 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32592232-E5EE-4474-A58C-6405B1D1FCD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6824159" y="5102039"/>
+          <a:ext cx="526170" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Inside</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1482,34 +3072,34 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1236669</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2741</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>278130</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>10360</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>94129</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129988</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F5A04A8-E12F-EFE1-66EA-484A826FC7A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB89671-C537-4008-9926-F9F2F8128D72}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="1"/>
+          <a:stCxn id="42" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="1581150" y="2670810"/>
-          <a:ext cx="899160" cy="82750"/>
+        <a:xfrm>
+          <a:off x="10205857" y="4780929"/>
+          <a:ext cx="1439296" cy="127247"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1537,32 +3127,34 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485888</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>37081</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>598170</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1036068</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>24877</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+        <xdr:cNvPr id="45" name="Straight Arrow Connector 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF98625-FEDD-4E1F-9E86-3730B7611BC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C13D8F8-4D2E-4ECD-8B87-513F68587AC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="43" idx="2"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3268980" y="2884170"/>
-          <a:ext cx="811530" cy="533400"/>
+          <a:off x="6537064" y="5366599"/>
+          <a:ext cx="550180" cy="722902"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1588,34 +3180,104 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>384363</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9637</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="681533" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="TextBox 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C86C294C-F179-47DF-B34B-BCC0B97801A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9272869" y="5706708"/>
+          <a:ext cx="681533" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Centroid</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>49306</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>94129</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>384363</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>141917</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+        <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B10396E-3995-4D24-9D79-F873B7069686}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CAB103E-D749-43D7-BE56-381CC67CE379}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3577590" y="3992880"/>
-          <a:ext cx="1135380" cy="182880"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9018494" y="5791200"/>
+          <a:ext cx="1787340" cy="415341"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1941,261 +3603,774 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FF3FA1-D90D-4839-866C-23521C09C0E6}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="12.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.20703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.15625" customWidth="1"/>
-    <col min="11" max="11" width="20.05078125" customWidth="1"/>
-    <col min="12" max="12" width="15.578125" customWidth="1"/>
+    <col min="11" max="11" width="21.15625" customWidth="1"/>
+    <col min="12" max="12" width="20.05078125" customWidth="1"/>
+    <col min="13" max="13" width="15.578125" customWidth="1"/>
+    <col min="14" max="14" width="15.05078125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>356</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-13389.373</v>
+      </c>
+      <c r="C2">
+        <v>3.5609126099999999</v>
+      </c>
+      <c r="D2">
+        <v>3.5</v>
+      </c>
+      <c r="E2">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>15745</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-10427.089</v>
+      </c>
+      <c r="C3">
+        <v>3.54642057</v>
+      </c>
+      <c r="D3">
+        <v>3.5699999299999998</v>
+      </c>
+      <c r="E3">
+        <v>9.375E-2</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
+        <v>8563.3739999999998</v>
+      </c>
+      <c r="K3" s="3">
+        <v>10518.687</v>
+      </c>
+      <c r="L3" s="8">
+        <v>10403.6</v>
+      </c>
+      <c r="M3" s="4">
+        <f>(J3-L3)/L3</f>
+        <v>-0.17688357876119809</v>
+      </c>
+      <c r="N3" s="4">
+        <f>(K3-L3)/L3</f>
+        <v>1.1062228459379401E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1333</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-7509.11</v>
+      </c>
+      <c r="C4">
+        <v>3.5319278199999999</v>
+      </c>
+      <c r="D4">
+        <v>3.63999987</v>
+      </c>
+      <c r="E4">
+        <v>9.375E-2</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
+      <c r="J4" s="3">
+        <v>-1315.2650000000001</v>
+      </c>
+      <c r="K4" s="3">
+        <v>-1133.2280000000001</v>
+      </c>
+      <c r="L4" s="8">
+        <v>-1047.9000000000001</v>
+      </c>
+      <c r="M4" s="4">
+        <f>(J4-L4)/L4</f>
+        <v>0.25514362057448231</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N5" si="0">(K4-L4)/L4</f>
+        <v>8.1427617139039954E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>9640</v>
-      </c>
-      <c r="B2" s="1">
-        <v>61551512</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>35</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2">
-        <v>61550000</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="8" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>9529</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-4329.308</v>
+      </c>
+      <c r="C5">
+        <v>3.54517579</v>
+      </c>
+      <c r="D5">
+        <v>3.7229833600000002</v>
+      </c>
+      <c r="E5">
+        <v>9.375E-2</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>9</v>
+      <c r="J5" s="3">
+        <v>-13389.373</v>
+      </c>
+      <c r="K5" s="3">
+        <v>-13381.357</v>
+      </c>
+      <c r="L5" s="8">
+        <v>-13884.9</v>
+      </c>
+      <c r="M5" s="4">
+        <f>(J5-L5)/L5</f>
+        <v>-3.5688193649216056E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.6265511454889821E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>345</v>
-      </c>
-      <c r="B3" s="1">
-        <v>39901732</v>
-      </c>
-      <c r="C3">
-        <v>49.999996189999997</v>
-      </c>
-      <c r="D3">
-        <v>27.999998089999998</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="3">
-        <v>61551512</v>
-      </c>
-      <c r="K3" s="4">
-        <v>61550000</v>
-      </c>
-      <c r="L3" s="5">
-        <f>(J3-K3)/K3</f>
-        <v>2.4565393988627133E-5</v>
-      </c>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>1334</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-1315.2650000000001</v>
+      </c>
+      <c r="C6">
+        <v>3.5584230400000001</v>
+      </c>
+      <c r="D6">
+        <v>3.8059663800000001</v>
+      </c>
+      <c r="E6">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F6" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>8447</v>
-      </c>
-      <c r="B4" s="1">
-        <v>29080782</v>
-      </c>
-      <c r="C4">
-        <v>49.999988559999998</v>
-      </c>
-      <c r="D4">
-        <v>24.499998089999998</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="3">
-        <v>7432166.5</v>
-      </c>
-      <c r="K4" s="4">
-        <v>7430000</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" ref="L4:L5" si="0">(J4-K4)/K4</f>
-        <v>2.9158815612382233E-4</v>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>9524</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1263.357</v>
+      </c>
+      <c r="C7">
+        <v>3.54792833</v>
+      </c>
+      <c r="D7">
+        <v>3.8873774999999999</v>
+      </c>
+      <c r="E7">
+        <v>9.375E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>344</v>
-      </c>
-      <c r="B5" s="1">
-        <v>18256932</v>
-      </c>
-      <c r="C5">
-        <v>49.99998093</v>
-      </c>
-      <c r="D5">
-        <v>20.999996190000001</v>
-      </c>
-      <c r="E5">
-        <v>25</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="3">
-        <v>-46696284</v>
-      </c>
-      <c r="K5" s="4">
-        <v>-46700000</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="0"/>
-        <v>-7.9571734475374726E-5</v>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>1335</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3834.5329999999999</v>
+      </c>
+      <c r="C8">
+        <v>3.5374336199999998</v>
+      </c>
+      <c r="D8">
+        <v>3.9687883899999998</v>
+      </c>
+      <c r="E8">
+        <v>9.375E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>8455</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7432166.5</v>
-      </c>
-      <c r="C6">
-        <v>49.999977110000003</v>
-      </c>
-      <c r="D6">
-        <v>17.499998089999998</v>
-      </c>
-      <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>7430000</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>9515</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5197.3469999999998</v>
+      </c>
+      <c r="C9">
+        <v>3.5346803699999998</v>
+      </c>
+      <c r="D9">
+        <v>4.0143942800000003</v>
+      </c>
+      <c r="E9">
+        <v>9.375E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <v>343</v>
-      </c>
-      <c r="B7" s="1">
-        <v>-3393733.5</v>
-      </c>
-      <c r="C7">
-        <v>49.999973300000001</v>
-      </c>
-      <c r="D7">
-        <v>13.99999809</v>
-      </c>
-      <c r="E7">
-        <v>25</v>
-      </c>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>14708</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8563.3739999999998</v>
+      </c>
+      <c r="C10">
+        <v>3.54642057</v>
+      </c>
+      <c r="D10">
+        <v>4.1300001100000001</v>
+      </c>
+      <c r="E10">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F10" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>8463</v>
-      </c>
-      <c r="B8" s="1">
-        <v>-14221835</v>
-      </c>
-      <c r="C8">
-        <v>49.999984740000002</v>
-      </c>
-      <c r="D8">
-        <v>10.49999905</v>
-      </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>342</v>
-      </c>
-      <c r="B9" s="1">
-        <v>-25048874</v>
-      </c>
-      <c r="C9">
-        <v>49.999996189999997</v>
-      </c>
-      <c r="D9">
-        <v>6.9999976200000003</v>
-      </c>
-      <c r="E9">
-        <v>25</v>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-13381.357</v>
+      </c>
+      <c r="C13">
+        <v>3.5609126099999999</v>
+      </c>
+      <c r="D13">
+        <v>3.5</v>
+      </c>
+      <c r="E13">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-13389.373</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>10129</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-46696284</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2">
-        <v>-46700000</v>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>11470</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-13219.883</v>
+      </c>
+      <c r="C14">
+        <v>3.5616011599999999</v>
+      </c>
+      <c r="D14">
+        <v>3.5037961000000002</v>
+      </c>
+      <c r="E14">
+        <v>9.375E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="1"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>834</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-13046.843999999999</v>
+      </c>
+      <c r="C15">
+        <v>3.56228948</v>
+      </c>
+      <c r="D15">
+        <v>3.5075919600000001</v>
+      </c>
+      <c r="E15">
+        <v>9.375E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="1"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>11456</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-12790.731</v>
+      </c>
+      <c r="C16">
+        <v>3.5622575300000001</v>
+      </c>
+      <c r="D16">
+        <v>3.5132603599999999</v>
+      </c>
+      <c r="E16">
+        <v>9.375E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="1"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>923</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-12522.108</v>
+      </c>
+      <c r="C17">
+        <v>3.5622255799999998</v>
+      </c>
+      <c r="D17">
+        <v>3.518929</v>
+      </c>
+      <c r="E17">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>11765</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-12099.148999999999</v>
+      </c>
+      <c r="C18">
+        <v>3.56268764</v>
+      </c>
+      <c r="D18">
+        <v>3.5282106400000002</v>
+      </c>
+      <c r="E18">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>965</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-11326.541999999999</v>
+      </c>
+      <c r="C19">
+        <v>3.5622653999999998</v>
+      </c>
+      <c r="D19">
+        <v>3.5453324300000002</v>
+      </c>
+      <c r="E19">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>10519</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-10483.416999999999</v>
+      </c>
+      <c r="C20">
+        <v>3.5627181499999998</v>
+      </c>
+      <c r="D20">
+        <v>3.5645408600000001</v>
+      </c>
+      <c r="E20">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-10427.089</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>990</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-9087.8610000000008</v>
+      </c>
+      <c r="C21">
+        <v>3.5605185000000001</v>
+      </c>
+      <c r="D21">
+        <v>3.5975379900000002</v>
+      </c>
+      <c r="E21">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>9025</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-6866.0330000000004</v>
+      </c>
+      <c r="C22">
+        <v>3.5587611199999998</v>
+      </c>
+      <c r="D22">
+        <v>3.6529176200000002</v>
+      </c>
+      <c r="E22">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-7509.11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>10288</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-4565.4790000000003</v>
+      </c>
+      <c r="C23">
+        <v>3.5664246099999999</v>
+      </c>
+      <c r="D23">
+        <v>3.7133224</v>
+      </c>
+      <c r="E23">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>-4329.308</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>10289</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-2668.4749999999999</v>
+      </c>
+      <c r="C24">
+        <v>3.5621850500000001</v>
+      </c>
+      <c r="D24">
+        <v>3.7666833400000002</v>
+      </c>
+      <c r="E24">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>5901</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-1133.2280000000001</v>
+      </c>
+      <c r="C25">
+        <v>3.5453202699999999</v>
+      </c>
+      <c r="D25">
+        <v>3.8135280599999999</v>
+      </c>
+      <c r="E25">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>-1315.2650000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>11058</v>
+      </c>
+      <c r="B26" s="1">
+        <v>636.24800000000005</v>
+      </c>
+      <c r="C26">
+        <v>3.53823066</v>
+      </c>
+      <c r="D26">
+        <v>3.8675391700000001</v>
+      </c>
+      <c r="E26">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1263.357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>997</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4580.3410000000003</v>
+      </c>
+      <c r="C27">
+        <v>3.5682056000000002</v>
+      </c>
+      <c r="D27">
+        <v>3.9920864100000002</v>
+      </c>
+      <c r="E27">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3834.5329999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>8989</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5463.5150000000003</v>
+      </c>
+      <c r="C28">
+        <v>3.5633132500000002</v>
+      </c>
+      <c r="D28">
+        <v>4.0221362100000002</v>
+      </c>
+      <c r="E28">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5197.3469999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>998</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6350.9669999999996</v>
+      </c>
+      <c r="C29">
+        <v>3.5584209000000002</v>
+      </c>
+      <c r="D29">
+        <v>4.05218554</v>
+      </c>
+      <c r="E29">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>7136</v>
+      </c>
+      <c r="B30" s="1">
+        <v>7070.3389999999999</v>
+      </c>
+      <c r="C30">
+        <v>3.5581207300000002</v>
+      </c>
+      <c r="D30">
+        <v>4.0769815400000002</v>
+      </c>
+      <c r="E30">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>991</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7785.4579999999996</v>
+      </c>
+      <c r="C31">
+        <v>3.5578205600000001</v>
+      </c>
+      <c r="D31">
+        <v>4.1017770799999997</v>
+      </c>
+      <c r="E31">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>9971</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8804.7759999999998</v>
+      </c>
+      <c r="C32">
+        <v>3.5588183400000002</v>
+      </c>
+      <c r="D32">
+        <v>4.1376342800000003</v>
+      </c>
+      <c r="E32">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>8563.3739999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>966</v>
+      </c>
+      <c r="B33" s="1">
+        <v>9378.8680000000004</v>
+      </c>
+      <c r="C33">
+        <v>3.55984831</v>
+      </c>
+      <c r="D33">
+        <v>4.1581554399999998</v>
+      </c>
+      <c r="E33">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>9849</v>
+      </c>
+      <c r="B34" s="1">
+        <v>9682.51</v>
+      </c>
+      <c r="C34">
+        <v>3.5599348499999999</v>
+      </c>
+      <c r="D34">
+        <v>4.1690969500000001</v>
+      </c>
+      <c r="E34">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>922</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9986.1350000000002</v>
+      </c>
+      <c r="C35">
+        <v>3.5600218799999999</v>
+      </c>
+      <c r="D35">
+        <v>4.1800375000000001</v>
+      </c>
+      <c r="E35">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>7939</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10146.768</v>
+      </c>
+      <c r="C36">
+        <v>3.5608963999999999</v>
+      </c>
+      <c r="D36">
+        <v>4.1860923799999998</v>
+      </c>
+      <c r="E36">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>788</v>
+      </c>
+      <c r="B37" s="1">
+        <v>10301.344999999999</v>
+      </c>
+      <c r="C37">
+        <v>3.5617709199999998</v>
+      </c>
+      <c r="D37">
+        <v>4.1921472499999997</v>
+      </c>
+      <c r="E37">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>5829</v>
+      </c>
+      <c r="B38" s="1">
+        <v>10410.376</v>
+      </c>
+      <c r="C38">
+        <v>3.5613417599999999</v>
+      </c>
+      <c r="D38">
+        <v>4.1960735299999996</v>
+      </c>
+      <c r="E38">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>28</v>
+      </c>
+      <c r="B39" s="1">
+        <v>10518.687</v>
+      </c>
+      <c r="C39">
+        <v>3.5609126099999999</v>
+      </c>
+      <c r="D39">
+        <v>4.1999998099999996</v>
+      </c>
+      <c r="E39">
+        <v>9.375E-2</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:E12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>